<commit_message>
Auto stash before rebase of "CarolinaCasillas/main"
Proyecto completo
</commit_message>
<xml_diff>
--- a/Datos Ajuste de Curvas.xlsx
+++ b/Datos Ajuste de Curvas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ea63f55690cd23a/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/francisco_balcazar_iteso_mx/Documents/Documentos ITESO/TAREA ITESO/3er Semestre/Simulacion Matematica/Proyecto 1/PM1_BalcazarF1_CasillasC2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD50BE08-8BFB-41DB-8B8C-972652A46F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{BD50BE08-8BFB-41DB-8B8C-972652A46F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDCD1C6-0BB1-46AC-8606-BBA767B531DE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0A34414C-695D-4928-BD7D-363B2DEBCF9B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A34414C-695D-4928-BD7D-363B2DEBCF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,12 +73,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,179 +409,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DCBA7FB-90FE-4ACD-8D16-17D2D8AA4D2B}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="C4:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
         <v>2019</v>
       </c>
-      <c r="B2">
+      <c r="D5" s="1">
         <v>146.75800000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="1">
         <v>2018</v>
       </c>
-      <c r="B3">
+      <c r="D6" s="1">
         <v>145.84</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="1">
         <v>2017</v>
       </c>
-      <c r="B4">
+      <c r="D7" s="1">
         <v>129.70500000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
         <v>2016</v>
       </c>
-      <c r="B5">
+      <c r="D8" s="1">
         <v>117.473</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="1">
         <v>2015</v>
       </c>
-      <c r="B6">
+      <c r="D9" s="1">
         <v>105.57299999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
         <v>2014</v>
       </c>
-      <c r="B7">
+      <c r="D10" s="1">
         <v>100.28400000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
         <v>2013</v>
       </c>
-      <c r="B8">
+      <c r="D11" s="1">
         <v>98.361000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
         <v>2012</v>
       </c>
-      <c r="B9">
+      <c r="D12" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
         <v>2011</v>
       </c>
-      <c r="B10">
+      <c r="D13" s="1">
         <v>96.57</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
         <v>2010</v>
       </c>
-      <c r="B11">
+      <c r="D14" s="1">
         <v>90.114999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
         <v>2009</v>
       </c>
-      <c r="B12">
+      <c r="D15" s="1">
         <v>86.36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
         <v>2008</v>
       </c>
-      <c r="B13">
+      <c r="D16" s="1">
         <v>92.426000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
         <v>2007</v>
       </c>
-      <c r="B14">
+      <c r="D17" s="1">
         <v>80.006</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
         <v>2006</v>
       </c>
-      <c r="B15">
+      <c r="D18" s="1">
         <v>81.525000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="1">
         <v>2005</v>
       </c>
-      <c r="B16">
+      <c r="D19" s="1">
         <v>69.623999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="1">
         <v>2004</v>
       </c>
-      <c r="B17">
+      <c r="D20" s="1">
         <v>73.852999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
         <v>2003</v>
       </c>
-      <c r="B18">
+      <c r="D21" s="1">
         <v>62.067</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
         <v>2002</v>
       </c>
-      <c r="B19">
+      <c r="D22" s="1">
         <v>56.323</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
         <v>2001</v>
       </c>
-      <c r="B20">
+      <c r="D23" s="1">
         <v>57.295000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
         <v>2000</v>
       </c>
-      <c r="B21">
+      <c r="D24" s="1">
         <v>54.41</v>
       </c>
     </row>

</xml_diff>